<commit_message>
better landing page on fetch
</commit_message>
<xml_diff>
--- a/excel_reports/EnlightNuUsaLLC_House.xlsx
+++ b/excel_reports/EnlightNuUsaLLC_House.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="210">
   <si>
     <t>Policy Record</t>
   </si>
@@ -285,6 +285,21 @@
     <t>04-01-2022</t>
   </si>
   <si>
+    <t>3173184837</t>
+  </si>
+  <si>
+    <t>6459551</t>
+  </si>
+  <si>
+    <t>Kim</t>
+  </si>
+  <si>
+    <t>Kellner</t>
+  </si>
+  <si>
+    <t>10-05-2021</t>
+  </si>
+  <si>
     <t>3173286698</t>
   </si>
   <si>
@@ -423,6 +438,36 @@
     <t>06-01-2022</t>
   </si>
   <si>
+    <t>3168411539</t>
+  </si>
+  <si>
+    <t>313301</t>
+  </si>
+  <si>
+    <t>Janice</t>
+  </si>
+  <si>
+    <t>Campbell</t>
+  </si>
+  <si>
+    <t>Advantage</t>
+  </si>
+  <si>
+    <t>500 - Cancelled</t>
+  </si>
+  <si>
+    <t>11-18-2020</t>
+  </si>
+  <si>
+    <t>01-01-2021</t>
+  </si>
+  <si>
+    <t>10-09-2022</t>
+  </si>
+  <si>
+    <t>12-31-2021</t>
+  </si>
+  <si>
     <t>3167039925</t>
   </si>
   <si>
@@ -441,18 +486,12 @@
     <t>AARP Medicare Advantage Choice (PPO)</t>
   </si>
   <si>
-    <t>Advantage</t>
-  </si>
-  <si>
     <t>410 - Cancelled</t>
   </si>
   <si>
     <t>10-28-2021</t>
   </si>
   <si>
-    <t>10-09-2022</t>
-  </si>
-  <si>
     <t>3798777905</t>
   </si>
   <si>
@@ -606,7 +645,7 @@
     <t>Copay - Commission:</t>
   </si>
   <si>
-    <t>15</t>
+    <t>18</t>
   </si>
 </sst>
 </file>
@@ -1013,35 +1052,35 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="B5" s="4">
         <f>B3+B4-B2</f>
@@ -1050,7 +1089,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="B6" s="2">
         <v>-30</v>
@@ -1058,30 +1097,30 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="B8" s="4">
         <f>SUM(B5:B7)</f>
         <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="B9" s="5">
         <f>MAX(0, B8*150)</f>
@@ -1090,12 +1129,12 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="B12" s="2">
         <v>0</v>
@@ -1103,7 +1142,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="B13" s="2">
         <v>0</v>
@@ -1111,20 +1150,20 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="4" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="B17" s="5">
         <f>SUM(Core!T:T)</f>
@@ -1133,12 +1172,12 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -1146,7 +1185,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -1154,7 +1193,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
       <c r="B22" s="2">
         <v>0</v>
@@ -1162,7 +1201,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="B23">
         <f>-B20+B21+B22</f>
@@ -1171,7 +1210,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="4" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="B24" s="5">
         <f>B23*50</f>
@@ -1180,17 +1219,17 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="B28" s="2">
         <v>0</v>
@@ -1198,7 +1237,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
       <c r="B29">
         <f>-B26+B27+B28</f>
@@ -1207,7 +1246,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="4" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="B30" s="5">
         <f>B29*100</f>
@@ -1221,7 +1260,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W52"/>
+  <dimension ref="A1:W56"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1685,7 +1724,13 @@
         <v>34</v>
       </c>
       <c r="S14" s="7" t="s">
-        <v>45</v>
+        <v>34</v>
+      </c>
+      <c r="T14" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="W14" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:23">
@@ -1735,7 +1780,13 @@
         <v>34</v>
       </c>
       <c r="S16" s="7" t="s">
-        <v>45</v>
+        <v>34</v>
+      </c>
+      <c r="T16" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="W16" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:23">
@@ -1914,10 +1965,10 @@
         <v>92</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>27</v>
@@ -1941,19 +1992,13 @@
         <v>93</v>
       </c>
       <c r="N24" t="s">
-        <v>93</v>
+        <v>44</v>
       </c>
       <c r="Q24" s="6" t="s">
         <v>34</v>
       </c>
       <c r="S24" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="T24" s="6">
-        <v>2.5</v>
-      </c>
-      <c r="W24" t="b">
-        <v>1</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:23">
@@ -1964,10 +2009,10 @@
         <v>95</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>27</v>
@@ -1994,10 +2039,10 @@
         <v>32</v>
       </c>
       <c r="M26" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="N26" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="Q26" s="6" t="s">
         <v>34</v>
@@ -2014,16 +2059,16 @@
     </row>
     <row r="28" spans="1:23">
       <c r="A28" s="9" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>27</v>
@@ -2050,10 +2095,10 @@
         <v>32</v>
       </c>
       <c r="M28" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="N28" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="Q28" s="6" t="s">
         <v>34</v>
@@ -2070,16 +2115,16 @@
     </row>
     <row r="30" spans="1:23">
       <c r="A30" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>27</v>
@@ -2106,10 +2151,10 @@
         <v>32</v>
       </c>
       <c r="M30" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="N30" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="Q30" s="6" t="s">
         <v>34</v>
@@ -2126,16 +2171,16 @@
     </row>
     <row r="32" spans="1:23">
       <c r="A32" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>27</v>
@@ -2162,30 +2207,36 @@
         <v>32</v>
       </c>
       <c r="M32" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="N32" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="Q32" s="6" t="s">
         <v>34</v>
       </c>
       <c r="S32" s="7" t="s">
-        <v>45</v>
+        <v>34</v>
+      </c>
+      <c r="T32" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="W32" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:23">
       <c r="A34" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>27</v>
@@ -2212,10 +2263,10 @@
         <v>32</v>
       </c>
       <c r="M34" t="s">
-        <v>112</v>
+        <v>69</v>
       </c>
       <c r="N34" t="s">
-        <v>112</v>
+        <v>69</v>
       </c>
       <c r="Q34" s="6" t="s">
         <v>34</v>
@@ -2232,13 +2283,13 @@
     </row>
     <row r="36" spans="1:23">
       <c r="A36" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>116</v>
@@ -2268,10 +2319,10 @@
         <v>32</v>
       </c>
       <c r="M36" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="N36" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="Q36" s="6" t="s">
         <v>34</v>
@@ -2288,16 +2339,16 @@
     </row>
     <row r="38" spans="1:23">
       <c r="A38" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>27</v>
@@ -2324,16 +2375,22 @@
         <v>32</v>
       </c>
       <c r="M38" t="s">
-        <v>121</v>
+        <v>83</v>
       </c>
       <c r="N38" t="s">
-        <v>121</v>
+        <v>83</v>
       </c>
       <c r="Q38" s="6" t="s">
         <v>34</v>
       </c>
       <c r="S38" s="7" t="s">
-        <v>45</v>
+        <v>34</v>
+      </c>
+      <c r="T38" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="W38" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:23">
@@ -2374,36 +2431,30 @@
         <v>32</v>
       </c>
       <c r="M40" t="s">
-        <v>83</v>
+        <v>126</v>
       </c>
       <c r="N40" t="s">
-        <v>83</v>
+        <v>126</v>
       </c>
       <c r="Q40" s="6" t="s">
         <v>34</v>
       </c>
       <c r="S40" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="T40" s="6">
-        <v>2.5</v>
-      </c>
-      <c r="W40" t="b">
-        <v>1</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:23">
       <c r="A42" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>27</v>
@@ -2430,10 +2481,10 @@
         <v>32</v>
       </c>
       <c r="M42" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="N42" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="Q42" s="6" t="s">
         <v>34</v>
@@ -2450,16 +2501,16 @@
     </row>
     <row r="44" spans="1:23">
       <c r="A44" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>27</v>
@@ -2486,16 +2537,22 @@
         <v>32</v>
       </c>
       <c r="M44" t="s">
-        <v>134</v>
+        <v>33</v>
       </c>
       <c r="N44" t="s">
-        <v>134</v>
+        <v>33</v>
       </c>
       <c r="Q44" s="6" t="s">
         <v>34</v>
       </c>
       <c r="S44" s="7" t="s">
-        <v>45</v>
+        <v>34</v>
+      </c>
+      <c r="T44" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="W44" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:23">
@@ -2512,160 +2569,166 @@
         <v>138</v>
       </c>
       <c r="E46" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K46" t="s">
+        <v>31</v>
+      </c>
+      <c r="L46" t="s">
+        <v>32</v>
+      </c>
+      <c r="M46" t="s">
+        <v>139</v>
+      </c>
+      <c r="N46" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q46" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S46" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23">
+      <c r="A48" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E48" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F46" s="6" t="s">
+      <c r="F48" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G46" s="6" t="s">
+      <c r="G48" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K48" t="s">
+        <v>144</v>
+      </c>
+      <c r="L48" t="s">
+        <v>145</v>
+      </c>
+      <c r="M48" t="s">
+        <v>146</v>
+      </c>
+      <c r="N48" t="s">
+        <v>147</v>
+      </c>
+      <c r="O48" t="s">
+        <v>148</v>
+      </c>
+      <c r="P48" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q48" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="S48" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19">
+      <c r="A50" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="E50" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="H46" s="6" t="s">
+      <c r="F50" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I46" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="J46" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="K46" t="s">
-        <v>141</v>
-      </c>
-      <c r="L46" t="s">
-        <v>142</v>
-      </c>
-      <c r="M46" t="s">
-        <v>143</v>
-      </c>
-      <c r="N46" t="s">
+      <c r="G50" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H50" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="K50" t="s">
+        <v>144</v>
+      </c>
+      <c r="L50" t="s">
+        <v>156</v>
+      </c>
+      <c r="M50" t="s">
+        <v>157</v>
+      </c>
+      <c r="N50" t="s">
         <v>44</v>
       </c>
-      <c r="O46" t="s">
-        <v>144</v>
-      </c>
-      <c r="P46" t="s">
+      <c r="O50" t="s">
+        <v>148</v>
+      </c>
+      <c r="P50" t="s">
         <v>44</v>
       </c>
-      <c r="Q46" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="47" spans="1:23">
-      <c r="A47" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H47" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I47" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="J47" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="K47" t="s">
-        <v>141</v>
-      </c>
-      <c r="L47" t="s">
-        <v>32</v>
-      </c>
-      <c r="M47" t="s">
-        <v>147</v>
-      </c>
-      <c r="N47" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q47" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="S47" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19">
-      <c r="A49" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H49" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I49" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="K49" t="s">
-        <v>141</v>
-      </c>
-      <c r="L49" t="s">
-        <v>32</v>
-      </c>
-      <c r="M49" t="s">
-        <v>44</v>
-      </c>
-      <c r="N49" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q49" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="S49" s="7" t="s">
-        <v>45</v>
+      <c r="Q50" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="51" spans="1:19">
       <c r="A51" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C51" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="D51" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="C51" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>155</v>
-      </c>
       <c r="E51" s="6" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="G51" s="6" t="s">
         <v>50</v>
@@ -2674,80 +2737,177 @@
         <v>51</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>139</v>
+        <v>154</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="K51" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="L51" t="s">
-        <v>142</v>
+        <v>32</v>
       </c>
       <c r="M51" t="s">
+        <v>160</v>
+      </c>
+      <c r="N51" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q51" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S51" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19">
+      <c r="A53" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H53" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I53" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="K53" t="s">
+        <v>144</v>
+      </c>
+      <c r="L53" t="s">
+        <v>32</v>
+      </c>
+      <c r="M53" t="s">
+        <v>44</v>
+      </c>
+      <c r="N53" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q53" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S53" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19">
+      <c r="A55" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I55" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="J55" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="K55" t="s">
+        <v>144</v>
+      </c>
+      <c r="L55" t="s">
         <v>156</v>
       </c>
-      <c r="N51" t="s">
-        <v>157</v>
-      </c>
-      <c r="O51" t="s">
+      <c r="M55" t="s">
+        <v>169</v>
+      </c>
+      <c r="N55" t="s">
+        <v>170</v>
+      </c>
+      <c r="O55" t="s">
+        <v>148</v>
+      </c>
+      <c r="P55" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q55" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19">
+      <c r="A56" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H56" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I56" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="J56" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="K56" t="s">
         <v>144</v>
       </c>
-      <c r="P51" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q51" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19">
-      <c r="A52" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G52" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H52" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I52" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="J52" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="K52" t="s">
-        <v>141</v>
-      </c>
-      <c r="L52" t="s">
+      <c r="L56" t="s">
         <v>32</v>
       </c>
-      <c r="M52" t="s">
-        <v>162</v>
-      </c>
-      <c r="N52" t="s">
+      <c r="M56" t="s">
+        <v>175</v>
+      </c>
+      <c r="N56" t="s">
         <v>88</v>
       </c>
-      <c r="Q52" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="S52" s="7" t="s">
+      <c r="Q56" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S56" s="7" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2799,14 +2959,18 @@
     <hyperlink ref="B44" r:id="rId44"/>
     <hyperlink ref="A46" r:id="rId45"/>
     <hyperlink ref="B46" r:id="rId46"/>
-    <hyperlink ref="A47" r:id="rId47"/>
-    <hyperlink ref="B47" r:id="rId48"/>
-    <hyperlink ref="A49" r:id="rId49"/>
-    <hyperlink ref="B49" r:id="rId50"/>
+    <hyperlink ref="A48" r:id="rId47"/>
+    <hyperlink ref="B48" r:id="rId48"/>
+    <hyperlink ref="A50" r:id="rId49"/>
+    <hyperlink ref="B50" r:id="rId50"/>
     <hyperlink ref="A51" r:id="rId51"/>
     <hyperlink ref="B51" r:id="rId52"/>
-    <hyperlink ref="A52" r:id="rId53"/>
-    <hyperlink ref="B52" r:id="rId54"/>
+    <hyperlink ref="A53" r:id="rId53"/>
+    <hyperlink ref="B53" r:id="rId54"/>
+    <hyperlink ref="A55" r:id="rId55"/>
+    <hyperlink ref="B55" r:id="rId56"/>
+    <hyperlink ref="A56" r:id="rId57"/>
+    <hyperlink ref="B56" r:id="rId58"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2887,7 +3051,7 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="9" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>47</v>
@@ -2911,13 +3075,13 @@
         <v>28</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="K2" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="L2" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
load data from data before generating reports
</commit_message>
<xml_diff>
--- a/excel_reports/EnlightNuUsaLLC_House.xlsx
+++ b/excel_reports/EnlightNuUsaLLC_House.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="199">
   <si>
     <t>Policy Record</t>
   </si>
@@ -285,21 +285,6 @@
     <t>04-01-2022</t>
   </si>
   <si>
-    <t>3173184837</t>
-  </si>
-  <si>
-    <t>6459551</t>
-  </si>
-  <si>
-    <t>Kim</t>
-  </si>
-  <si>
-    <t>Kellner</t>
-  </si>
-  <si>
-    <t>10-05-2021</t>
-  </si>
-  <si>
     <t>3173286698</t>
   </si>
   <si>
@@ -438,99 +423,51 @@
     <t>06-01-2022</t>
   </si>
   <si>
-    <t>3168411539</t>
-  </si>
-  <si>
-    <t>313301</t>
-  </si>
-  <si>
-    <t>Janice</t>
-  </si>
-  <si>
-    <t>Campbell</t>
+    <t>3167095955</t>
+  </si>
+  <si>
+    <t>16778215</t>
+  </si>
+  <si>
+    <t>Charles</t>
+  </si>
+  <si>
+    <t>Dudley</t>
+  </si>
+  <si>
+    <t>AARP/UHC</t>
   </si>
   <si>
     <t>Advantage</t>
   </si>
   <si>
-    <t>500 - Cancelled</t>
-  </si>
-  <si>
-    <t>11-18-2020</t>
-  </si>
-  <si>
-    <t>01-01-2021</t>
+    <t>3168434998</t>
+  </si>
+  <si>
+    <t>9263551</t>
+  </si>
+  <si>
+    <t>Norma</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>AARP Medicare Advantage Choice (PPO)</t>
+  </si>
+  <si>
+    <t>410 - Cancelled</t>
+  </si>
+  <si>
+    <t>01-25-2022</t>
+  </si>
+  <si>
+    <t>03-01-2022</t>
   </si>
   <si>
     <t>10-09-2022</t>
   </si>
   <si>
-    <t>12-31-2021</t>
-  </si>
-  <si>
-    <t>3167039925</t>
-  </si>
-  <si>
-    <t>6922601</t>
-  </si>
-  <si>
-    <t>Margaret(Peg)</t>
-  </si>
-  <si>
-    <t>Colyar</t>
-  </si>
-  <si>
-    <t>AARP/UHC</t>
-  </si>
-  <si>
-    <t>AARP Medicare Advantage Choice (PPO)</t>
-  </si>
-  <si>
-    <t>410 - Cancelled</t>
-  </si>
-  <si>
-    <t>10-28-2021</t>
-  </si>
-  <si>
-    <t>3798777905</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AARP MA Patriot </t>
-  </si>
-  <si>
-    <t>11-23-2021</t>
-  </si>
-  <si>
-    <t>3167095955</t>
-  </si>
-  <si>
-    <t>16778215</t>
-  </si>
-  <si>
-    <t>Charles</t>
-  </si>
-  <si>
-    <t>Dudley</t>
-  </si>
-  <si>
-    <t>3168434998</t>
-  </si>
-  <si>
-    <t>9263551</t>
-  </si>
-  <si>
-    <t>Norma</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>01-25-2022</t>
-  </si>
-  <si>
-    <t>03-01-2022</t>
-  </si>
-  <si>
     <t>03-31-2022</t>
   </si>
   <si>
@@ -546,6 +483,36 @@
     <t>03-24-2022</t>
   </si>
   <si>
+    <t>3167091334</t>
+  </si>
+  <si>
+    <t>6821051</t>
+  </si>
+  <si>
+    <t>Judson</t>
+  </si>
+  <si>
+    <t>Simon</t>
+  </si>
+  <si>
+    <t>CIGNA</t>
+  </si>
+  <si>
+    <t>Cigna Preferred Medicare (HMO)</t>
+  </si>
+  <si>
+    <t>11-05-2021</t>
+  </si>
+  <si>
+    <t>3799452754</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cigna Alliance Medicare (HMO) </t>
+  </si>
+  <si>
+    <t>12-07-2021</t>
+  </si>
+  <si>
     <t>3172447096</t>
   </si>
   <si>
@@ -645,7 +612,7 @@
     <t>Copay - Commission:</t>
   </si>
   <si>
-    <t>18</t>
+    <t>19</t>
   </si>
 </sst>
 </file>
@@ -1052,35 +1019,35 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="B5" s="4">
         <f>B3+B4-B2</f>
@@ -1089,7 +1056,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="B6" s="2">
         <v>-30</v>
@@ -1097,30 +1064,30 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B8" s="4">
         <f>SUM(B5:B7)</f>
         <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="B9" s="5">
         <f>MAX(0, B8*150)</f>
@@ -1129,12 +1096,12 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="B12" s="2">
         <v>0</v>
@@ -1142,7 +1109,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="B13" s="2">
         <v>0</v>
@@ -1150,20 +1117,20 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="4" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="B17" s="5">
         <f>SUM(Core!T:T)</f>
@@ -1172,12 +1139,12 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -1185,7 +1152,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -1193,7 +1160,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="B22" s="2">
         <v>0</v>
@@ -1201,7 +1168,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="B23">
         <f>-B20+B21+B22</f>
@@ -1210,7 +1177,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="4" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="B24" s="5">
         <f>B23*50</f>
@@ -1219,17 +1186,17 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="B28" s="2">
         <v>0</v>
@@ -1237,7 +1204,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="B29">
         <f>-B26+B27+B28</f>
@@ -1246,7 +1213,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="4" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="B30" s="5">
         <f>B29*100</f>
@@ -1260,7 +1227,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W56"/>
+  <dimension ref="A1:W52"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1965,10 +1932,10 @@
         <v>92</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>27</v>
@@ -1992,13 +1959,19 @@
         <v>93</v>
       </c>
       <c r="N24" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="Q24" s="6" t="s">
         <v>34</v>
       </c>
       <c r="S24" s="7" t="s">
-        <v>45</v>
+        <v>34</v>
+      </c>
+      <c r="T24" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="W24" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:23">
@@ -2009,10 +1982,10 @@
         <v>95</v>
       </c>
       <c r="C26" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>27</v>
@@ -2039,10 +2012,10 @@
         <v>32</v>
       </c>
       <c r="M26" t="s">
-        <v>98</v>
+        <v>33</v>
       </c>
       <c r="N26" t="s">
-        <v>98</v>
+        <v>33</v>
       </c>
       <c r="Q26" s="6" t="s">
         <v>34</v>
@@ -2059,16 +2032,16 @@
     </row>
     <row r="28" spans="1:23">
       <c r="A28" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="D28" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>101</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>27</v>
@@ -2095,10 +2068,10 @@
         <v>32</v>
       </c>
       <c r="M28" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="N28" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="Q28" s="6" t="s">
         <v>34</v>
@@ -2115,16 +2088,16 @@
     </row>
     <row r="30" spans="1:23">
       <c r="A30" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="C30" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="D30" s="6" t="s">
         <v>104</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>105</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>27</v>
@@ -2151,10 +2124,10 @@
         <v>32</v>
       </c>
       <c r="M30" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="N30" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="Q30" s="6" t="s">
         <v>34</v>
@@ -2171,16 +2144,16 @@
     </row>
     <row r="32" spans="1:23">
       <c r="A32" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="C32" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="D32" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>109</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>27</v>
@@ -2207,10 +2180,10 @@
         <v>32</v>
       </c>
       <c r="M32" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="N32" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="Q32" s="6" t="s">
         <v>34</v>
@@ -2227,16 +2200,16 @@
     </row>
     <row r="34" spans="1:23">
       <c r="A34" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="C34" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>111</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>113</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>27</v>
@@ -2263,10 +2236,10 @@
         <v>32</v>
       </c>
       <c r="M34" t="s">
-        <v>69</v>
+        <v>112</v>
       </c>
       <c r="N34" t="s">
-        <v>69</v>
+        <v>112</v>
       </c>
       <c r="Q34" s="6" t="s">
         <v>34</v>
@@ -2283,13 +2256,13 @@
     </row>
     <row r="36" spans="1:23">
       <c r="A36" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="C36" s="6" t="s">
         <v>115</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>108</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>116</v>
@@ -2319,10 +2292,10 @@
         <v>32</v>
       </c>
       <c r="M36" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="N36" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="Q36" s="6" t="s">
         <v>34</v>
@@ -2339,16 +2312,16 @@
     </row>
     <row r="38" spans="1:23">
       <c r="A38" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="C38" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="D38" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>121</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>27</v>
@@ -2375,22 +2348,16 @@
         <v>32</v>
       </c>
       <c r="M38" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
       <c r="N38" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
       <c r="Q38" s="6" t="s">
         <v>34</v>
       </c>
       <c r="S38" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="T38" s="6">
-        <v>2.5</v>
-      </c>
-      <c r="W38" t="b">
-        <v>1</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:23">
@@ -2431,30 +2398,36 @@
         <v>32</v>
       </c>
       <c r="M40" t="s">
-        <v>126</v>
+        <v>83</v>
       </c>
       <c r="N40" t="s">
-        <v>126</v>
+        <v>83</v>
       </c>
       <c r="Q40" s="6" t="s">
         <v>34</v>
       </c>
       <c r="S40" s="7" t="s">
-        <v>45</v>
+        <v>34</v>
+      </c>
+      <c r="T40" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="W40" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:23">
       <c r="A42" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B42" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="C42" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="D42" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>130</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>27</v>
@@ -2481,10 +2454,10 @@
         <v>32</v>
       </c>
       <c r="M42" t="s">
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="N42" t="s">
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="Q42" s="6" t="s">
         <v>34</v>
@@ -2501,16 +2474,16 @@
     </row>
     <row r="44" spans="1:23">
       <c r="A44" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B44" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="C44" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="D44" s="6" t="s">
         <v>133</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>134</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>27</v>
@@ -2537,22 +2510,16 @@
         <v>32</v>
       </c>
       <c r="M44" t="s">
-        <v>33</v>
+        <v>134</v>
       </c>
       <c r="N44" t="s">
-        <v>33</v>
+        <v>134</v>
       </c>
       <c r="Q44" s="6" t="s">
         <v>34</v>
       </c>
       <c r="S44" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="T44" s="6">
-        <v>2.5</v>
-      </c>
-      <c r="W44" t="b">
-        <v>1</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:23">
@@ -2581,22 +2548,19 @@
         <v>28</v>
       </c>
       <c r="I46" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="J46" s="6" t="s">
-        <v>30</v>
+        <v>139</v>
       </c>
       <c r="K46" t="s">
-        <v>31</v>
+        <v>140</v>
       </c>
       <c r="L46" t="s">
         <v>32</v>
       </c>
       <c r="M46" t="s">
-        <v>139</v>
+        <v>44</v>
       </c>
       <c r="N46" t="s">
-        <v>139</v>
+        <v>44</v>
       </c>
       <c r="Q46" s="6" t="s">
         <v>34</v>
@@ -2607,16 +2571,16 @@
     </row>
     <row r="48" spans="1:23">
       <c r="A48" s="9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>50</v>
@@ -2625,110 +2589,107 @@
         <v>51</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>52</v>
+        <v>139</v>
+      </c>
+      <c r="J48" s="6" t="s">
+        <v>145</v>
       </c>
       <c r="K48" t="s">
+        <v>140</v>
+      </c>
+      <c r="L48" t="s">
+        <v>146</v>
+      </c>
+      <c r="M48" t="s">
+        <v>147</v>
+      </c>
+      <c r="N48" t="s">
+        <v>148</v>
+      </c>
+      <c r="O48" t="s">
+        <v>149</v>
+      </c>
+      <c r="P48" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q48" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23">
+      <c r="A49" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D49" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="L48" t="s">
-        <v>145</v>
-      </c>
-      <c r="M48" t="s">
-        <v>146</v>
-      </c>
-      <c r="N48" t="s">
-        <v>147</v>
-      </c>
-      <c r="O48" t="s">
-        <v>148</v>
-      </c>
-      <c r="P48" t="s">
-        <v>149</v>
-      </c>
-      <c r="Q48" s="6" t="s">
+      <c r="E49" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="K49" t="s">
+        <v>140</v>
+      </c>
+      <c r="L49" t="s">
+        <v>32</v>
+      </c>
+      <c r="M49" t="s">
+        <v>154</v>
+      </c>
+      <c r="N49" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q49" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S49" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="S48" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19">
-      <c r="A50" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="E50" s="6" t="s">
+    </row>
+    <row r="51" spans="1:23">
+      <c r="A51" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E51" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F50" s="6" t="s">
+      <c r="F51" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H50" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I50" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="J50" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="K50" t="s">
-        <v>144</v>
-      </c>
-      <c r="L50" t="s">
-        <v>156</v>
-      </c>
-      <c r="M50" t="s">
-        <v>157</v>
-      </c>
-      <c r="N50" t="s">
-        <v>44</v>
-      </c>
-      <c r="O50" t="s">
-        <v>148</v>
-      </c>
-      <c r="P50" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q50" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19">
-      <c r="A51" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="B51" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="G51" s="6" t="s">
         <v>50</v>
@@ -2737,178 +2698,84 @@
         <v>51</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="J51" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="K51" t="s">
+        <v>140</v>
+      </c>
+      <c r="L51" t="s">
+        <v>146</v>
+      </c>
+      <c r="M51" t="s">
+        <v>161</v>
+      </c>
+      <c r="N51" t="s">
+        <v>69</v>
+      </c>
+      <c r="O51" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q51" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23">
+      <c r="A52" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H52" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I52" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="K51" t="s">
-        <v>144</v>
-      </c>
-      <c r="L51" t="s">
+      <c r="J52" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="K52" t="s">
+        <v>140</v>
+      </c>
+      <c r="L52" t="s">
         <v>32</v>
       </c>
-      <c r="M51" t="s">
-        <v>160</v>
-      </c>
-      <c r="N51" t="s">
+      <c r="M52" t="s">
+        <v>164</v>
+      </c>
+      <c r="N52" t="s">
         <v>44</v>
       </c>
-      <c r="Q51" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="S51" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19">
-      <c r="A53" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="B53" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G53" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H53" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I53" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="K53" t="s">
-        <v>144</v>
-      </c>
-      <c r="L53" t="s">
-        <v>32</v>
-      </c>
-      <c r="M53" t="s">
-        <v>44</v>
-      </c>
-      <c r="N53" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q53" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="S53" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="55" spans="1:19">
-      <c r="A55" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G55" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H55" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I55" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="J55" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="K55" t="s">
-        <v>144</v>
-      </c>
-      <c r="L55" t="s">
-        <v>156</v>
-      </c>
-      <c r="M55" t="s">
-        <v>169</v>
-      </c>
-      <c r="N55" t="s">
-        <v>170</v>
-      </c>
-      <c r="O55" t="s">
-        <v>148</v>
-      </c>
-      <c r="P55" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q55" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19">
-      <c r="A56" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="B56" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G56" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H56" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I56" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="J56" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="K56" t="s">
-        <v>144</v>
-      </c>
-      <c r="L56" t="s">
-        <v>32</v>
-      </c>
-      <c r="M56" t="s">
-        <v>175</v>
-      </c>
-      <c r="N56" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q56" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="S56" s="7" t="s">
-        <v>45</v>
+      <c r="Q52" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S52" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="T52" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="W52" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2961,16 +2828,12 @@
     <hyperlink ref="B46" r:id="rId46"/>
     <hyperlink ref="A48" r:id="rId47"/>
     <hyperlink ref="B48" r:id="rId48"/>
-    <hyperlink ref="A50" r:id="rId49"/>
-    <hyperlink ref="B50" r:id="rId50"/>
+    <hyperlink ref="A49" r:id="rId49"/>
+    <hyperlink ref="B49" r:id="rId50"/>
     <hyperlink ref="A51" r:id="rId51"/>
     <hyperlink ref="B51" r:id="rId52"/>
-    <hyperlink ref="A53" r:id="rId53"/>
-    <hyperlink ref="B53" r:id="rId54"/>
-    <hyperlink ref="A55" r:id="rId55"/>
-    <hyperlink ref="B55" r:id="rId56"/>
-    <hyperlink ref="A56" r:id="rId57"/>
-    <hyperlink ref="B56" r:id="rId58"/>
+    <hyperlink ref="A52" r:id="rId53"/>
+    <hyperlink ref="B52" r:id="rId54"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3051,7 +2914,7 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="9" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>47</v>
@@ -3075,13 +2938,13 @@
         <v>28</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="K2" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="L2" t="s">
         <v>32</v>

</xml_diff>